<commit_message>
gerando arquivos de dados em txt para análise no R
</commit_message>
<xml_diff>
--- a/Data/Processed/01_Behavioral-Data_Acoustic-Exp.xlsx
+++ b/Data/Processed/01_Behavioral-Data_Acoustic-Exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Mestrado\Projeto\Artigos\Experimento\BESocio\Article_behav-S.max_V03\Data\Processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B593C1-4591-43A7-8BFE-A540154B25EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA23271-B0BF-47F5-A34B-23D0BA721756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="423" xr2:uid="{142E5FC4-F098-4765-975A-8B305CB69989}"/>
+    <workbookView xWindow="405" yWindow="165" windowWidth="14520" windowHeight="10635" tabRatio="423" xr2:uid="{142E5FC4-F098-4765-975A-8B305CB69989}"/>
   </bookViews>
   <sheets>
     <sheet name="Acoustic.model" sheetId="3" r:id="rId1"/>
@@ -182,16 +182,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,7 +213,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +532,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D97" sqref="D97:D101"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,32 +540,32 @@
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -582,43 +574,43 @@
       <c r="K1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Y1" s="1" t="s">

</xml_diff>